<commit_message>
:sparkles: Update copySheet method implementation
</commit_message>
<xml_diff>
--- a/sample/output-97-2007.xlsx
+++ b/sample/output-97-2007.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30480" windowHeight="24220"/>
+    <workbookView windowWidth="30480" windowHeight="24220" activeTab="0"/>
   </bookViews>
   <sheets>
+    <sheet name="copied_sheet" r:id="rId5" sheetId="2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet0" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t>基本信息</t>
   </si>
@@ -77,10 +77,175 @@
     <t>求和</t>
   </si>
   <si>
-    <t>旧文档</t>
-  </si>
-  <si>
-    <t>平均数</t>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>旧</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>档</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>多</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="53"/>
+        <sz val="11.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="53"/>
+        <sz val="11.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>本</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="53"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>在</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="10"/>
+        <sz val="22.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>一</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个</t>
+    </r>
+    <r>
+      <t>Cell</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>里</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>求</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>平</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>均</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="none"/>
+        <color indexed="8"/>
+        <sz val="12.0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>数</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -93,7 +258,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="53">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,6 +491,20 @@
     </font>
     <font>
       <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <color indexed="53"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="53"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
       <sz val="11.0"/>
       <u val="none"/>
       <color indexed="8"/>
@@ -345,6 +524,111 @@
       <b val="true"/>
       <u val="none"/>
       <color indexed="54"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="16"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="9"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <u val="none"/>
+      <color indexed="23"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="17"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="20"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="15.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="54"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="19"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="54"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="8"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="10"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="53"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="63"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="62"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="9"/>
       <charset val="134"/>
     </font>
     <font>
@@ -358,105 +642,14 @@
       <name val="宋体"/>
       <sz val="11.0"/>
       <u val="none"/>
-      <color indexed="9"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="15.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="54"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="18.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="54"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
       <color indexed="53"/>
       <charset val="134"/>
     </font>
     <font>
       <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="20"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <i val="true"/>
-      <u val="none"/>
-      <color indexed="23"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="8"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="63"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="9"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="16"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="17"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="53"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
+      <sz val="22.0"/>
       <u val="none"/>
       <color indexed="10"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="62"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -987,7 +1180,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1020,6 +1213,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="general" vertical="center" wrapText="false"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="general" vertical="center" wrapText="false"/>
@@ -1669,7 +1865,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1742,126 +1938,129 @@
       <c r="B13" s="22" t="n">
         <v>12.0</v>
       </c>
+      <c r="G13" s="23" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14">
-      <c r="B14" s="23" t="n">
+      <c r="B14" s="24" t="n">
         <v>13.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="25" t="n">
         <v>14.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="25" t="n">
+      <c r="B16" s="26" t="n">
         <v>15.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="26" t="n">
+      <c r="B17" s="27" t="n">
         <v>16.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="27" t="n">
+      <c r="B18" s="28" t="n">
         <v>17.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="28" t="n">
+      <c r="B19" s="29" t="n">
         <v>18.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="29" t="n">
+      <c r="B20" s="30" t="n">
         <v>19.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="30" t="n">
+      <c r="B21" s="31" t="n">
         <v>20.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="31" t="n">
+      <c r="B22" s="32" t="n">
         <v>21.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="32" t="n">
+      <c r="B23" s="33" t="n">
         <v>22.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="33" t="n">
+      <c r="B24" s="34" t="n">
         <v>23.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="34" t="n">
+      <c r="B25" s="35" t="n">
         <v>24.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="35" t="n">
+      <c r="B26" s="36" t="n">
         <v>25.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="36" t="n">
+      <c r="B27" s="37" t="n">
         <v>26.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="37" t="n">
+      <c r="B28" s="38" t="n">
         <v>27.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="38" t="n">
+      <c r="B29" s="39" t="n">
         <v>28.0</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="39" t="n">
+      <c r="B30" s="40" t="n">
         <v>29.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="40" t="n">
+      <c r="B31" s="41" t="n">
         <v>30.0</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="41" t="n">
+      <c r="B32" s="42" t="n">
         <v>31.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="42" t="n">
+      <c r="B33" s="43" t="n">
         <v>32.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="43" t="n">
+      <c r="B34" s="44" t="n">
         <v>33.0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="45" t="n">
+      <c r="A35" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="46" t="n">
         <f>SUM(B2:B34)</f>
         <v>561.0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="47" t="n">
+      <c r="A36" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="48" t="n">
         <f>AVERAGE(B2:B34)</f>
         <v>17.0</v>
       </c>

</xml_diff>